<commit_message>
Update Excel with correct images and force re-seed
</commit_message>
<xml_diff>
--- a/Pamorya Stock(1).xlsx
+++ b/Pamorya Stock(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amant\PycharmProjects\PythonProject1\NewChatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amant\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62890877-ADC9-4437-8E36-80EC3B72BB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D09F5-5F68-48BF-96C9-9D8BF4E67258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -333,73 +333,73 @@
     <t>image_url</t>
   </si>
   <si>
-    <t>http://localhost:8000/product_images/PCCS05.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PCR04.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PWBW01.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PPR02.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PPDCC03.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PEWE06.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PPDC07.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PSPG08.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PRRR09.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PCC010.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PMVD011.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PCC012.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PSW013.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PSH014.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PMW015.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PSROS016.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PGWM017.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PEA018.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PFB019.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PVV020.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PMSB021.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PMSP021.jpg</t>
-  </si>
-  <si>
-    <t>http://localhost:8000/product_images/PRB022.jpg</t>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PWBW01.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PPR02.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PPDCC03.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PCR04.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PCCS05.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PEWE06.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PPDC07.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PSPG08.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PRB022.jpg/PRRR09.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PCC010.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PMVD011.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PCC012.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PSW013.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PSH014.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PMW015.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PSROS016.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PGWM017.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PEA018.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PFB019.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PVV020.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PMSB021.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PMSP021.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dkftnrrjq/image/upload/v1765694935/apparel_bot_products/PRB022.jpg</t>
   </si>
 </sst>
 </file>
@@ -528,6 +528,43 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -539,45 +576,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -875,19 +875,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -896,7 +896,7 @@
       <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="25" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="2"/>
@@ -905,18 +905,18 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="27" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -933,7 +933,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>11</v>
@@ -953,19 +953,19 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -983,11 +983,11 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1003,11 +1003,11 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
@@ -1023,11 +1023,11 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="6" t="s">
         <v>20</v>
       </c>
@@ -1043,17 +1043,17 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
         <v>82</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1071,11 +1071,11 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1091,11 +1091,11 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="18"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1111,11 +1111,11 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="18"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1131,19 +1131,19 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="29.25" customHeight="1">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>83</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1161,11 +1161,11 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1181,11 +1181,11 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1201,11 +1201,11 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="6" t="s">
         <v>20</v>
       </c>
@@ -1221,19 +1221,19 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="24" customHeight="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>84</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1251,11 +1251,11 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1271,11 +1271,11 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1291,11 +1291,11 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="6" t="s">
         <v>20</v>
       </c>
@@ -1311,17 +1311,17 @@
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="17" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="14" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="6" t="s">
@@ -1339,11 +1339,11 @@
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1359,11 +1359,11 @@
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1379,11 +1379,11 @@
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1399,19 +1399,19 @@
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="D24" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>86</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1429,11 +1429,11 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="6" t="s">
         <v>18</v>
       </c>
@@ -1449,11 +1449,11 @@
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="6" t="s">
         <v>19</v>
       </c>
@@ -1469,11 +1469,11 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="6" t="s">
         <v>20</v>
       </c>
@@ -1489,19 +1489,19 @@
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="14" t="s">
         <v>87</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -1519,11 +1519,11 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="17"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="6" t="s">
         <v>18</v>
       </c>
@@ -1539,11 +1539,11 @@
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="17"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="6" t="s">
         <v>19</v>
       </c>
@@ -1559,11 +1559,11 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="17"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="6" t="s">
         <v>20</v>
       </c>
@@ -1579,19 +1579,19 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="14" t="s">
         <v>88</v>
       </c>
       <c r="F32" s="6" t="s">
@@ -1609,11 +1609,11 @@
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A33" s="30"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="17"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="6" t="s">
         <v>18</v>
       </c>
@@ -1629,11 +1629,11 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="17"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="6" t="s">
         <v>19</v>
       </c>
@@ -1649,11 +1649,11 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A35" s="30"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="17"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
       <c r="F35" s="6" t="s">
         <v>20</v>
       </c>
@@ -1669,19 +1669,19 @@
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="14" t="s">
         <v>89</v>
       </c>
       <c r="F36" s="6" t="s">
@@ -1699,11 +1699,11 @@
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A37" s="30"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="17"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="14"/>
       <c r="F37" s="6" t="s">
         <v>18</v>
       </c>
@@ -1719,11 +1719,11 @@
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="17"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="14"/>
       <c r="F38" s="6" t="s">
         <v>19</v>
       </c>
@@ -1739,11 +1739,11 @@
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A39" s="30"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="17"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="6" t="s">
         <v>20</v>
       </c>
@@ -1759,19 +1759,19 @@
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="14" t="s">
         <v>90</v>
       </c>
       <c r="F40" s="6" t="s">
@@ -1789,11 +1789,11 @@
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A41" s="30"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="17"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="6" t="s">
         <v>18</v>
       </c>
@@ -1809,11 +1809,11 @@
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A42" s="30"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="17"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="14"/>
       <c r="F42" s="6" t="s">
         <v>19</v>
       </c>
@@ -1829,11 +1829,11 @@
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="17"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="14"/>
       <c r="F43" s="6" t="s">
         <v>20</v>
       </c>
@@ -1849,19 +1849,19 @@
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -1879,11 +1879,11 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="17"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="6" t="s">
         <v>18</v>
       </c>
@@ -1899,11 +1899,11 @@
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A46" s="30"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="17"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14"/>
       <c r="F46" s="6" t="s">
         <v>19</v>
       </c>
@@ -1919,11 +1919,11 @@
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="17"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="6" t="s">
         <v>20</v>
       </c>
@@ -1939,19 +1939,19 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="14" t="s">
         <v>92</v>
       </c>
       <c r="F48" s="6" t="s">
@@ -1969,11 +1969,11 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A49" s="30"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="17"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="14"/>
       <c r="F49" s="6" t="s">
         <v>18</v>
       </c>
@@ -1989,11 +1989,11 @@
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A50" s="30"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="17"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="14"/>
       <c r="F50" s="6" t="s">
         <v>19</v>
       </c>
@@ -2009,11 +2009,11 @@
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A51" s="30"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="17"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="6" t="s">
         <v>20</v>
       </c>
@@ -2029,19 +2029,19 @@
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="14" t="s">
         <v>93</v>
       </c>
       <c r="F52" s="6" t="s">
@@ -2059,11 +2059,11 @@
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A53" s="30"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="17"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="6" t="s">
         <v>18</v>
       </c>
@@ -2079,11 +2079,11 @@
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A54" s="30"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="17"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="14"/>
       <c r="F54" s="6" t="s">
         <v>19</v>
       </c>
@@ -2099,11 +2099,11 @@
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A55" s="30"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="17"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="14"/>
       <c r="F55" s="6" t="s">
         <v>20</v>
       </c>
@@ -2119,19 +2119,19 @@
       <c r="L55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="14" t="s">
         <v>94</v>
       </c>
       <c r="F56" s="6" t="s">
@@ -2149,11 +2149,11 @@
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A57" s="30"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="17"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="14"/>
       <c r="F57" s="6" t="s">
         <v>18</v>
       </c>
@@ -2169,11 +2169,11 @@
       <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A58" s="30"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="17"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="14"/>
       <c r="F58" s="6" t="s">
         <v>19</v>
       </c>
@@ -2189,11 +2189,11 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A59" s="30"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="17"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="6" t="s">
         <v>20</v>
       </c>
@@ -2209,19 +2209,19 @@
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="14" t="s">
         <v>95</v>
       </c>
       <c r="F60" s="6" t="s">
@@ -2239,11 +2239,11 @@
       <c r="L60" s="1"/>
     </row>
     <row r="61" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A61" s="30"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="17"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="6" t="s">
         <v>18</v>
       </c>
@@ -2259,11 +2259,11 @@
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A62" s="30"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="17"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="6" t="s">
         <v>19</v>
       </c>
@@ -2279,11 +2279,11 @@
       <c r="L62" s="1"/>
     </row>
     <row r="63" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A63" s="30"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="17"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="6" t="s">
         <v>20</v>
       </c>
@@ -2299,19 +2299,19 @@
       <c r="L63" s="1"/>
     </row>
     <row r="64" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E64" s="14" t="s">
         <v>96</v>
       </c>
       <c r="F64" s="6" t="s">
@@ -2329,11 +2329,11 @@
       <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A65" s="30"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="17"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="6" t="s">
         <v>18</v>
       </c>
@@ -2349,11 +2349,11 @@
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A66" s="30"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="17"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="14"/>
       <c r="F66" s="6" t="s">
         <v>19</v>
       </c>
@@ -2369,11 +2369,11 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A67" s="30"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="17"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="14"/>
       <c r="F67" s="6" t="s">
         <v>20</v>
       </c>
@@ -2389,19 +2389,19 @@
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A68" s="30" t="s">
+      <c r="A68" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="20" t="s">
         <v>60</v>
       </c>
       <c r="F68" s="6" t="s">
@@ -2419,11 +2419,11 @@
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A69" s="30"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="28"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="20"/>
       <c r="F69" s="6" t="s">
         <v>18</v>
       </c>
@@ -2439,11 +2439,11 @@
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A70" s="30"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="28"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="20"/>
       <c r="F70" s="6" t="s">
         <v>19</v>
       </c>
@@ -2459,11 +2459,11 @@
       <c r="L70" s="1"/>
     </row>
     <row r="71" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A71" s="30"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="28"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="20"/>
       <c r="F71" s="6" t="s">
         <v>20</v>
       </c>
@@ -2479,19 +2479,19 @@
       <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A72" s="30" t="s">
+      <c r="A72" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D72" s="19" t="s">
+      <c r="D72" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="15" t="s">
         <v>63</v>
       </c>
       <c r="F72" s="6" t="s">
@@ -2509,11 +2509,11 @@
       <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A73" s="30"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="29"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="15"/>
       <c r="F73" s="6" t="s">
         <v>18</v>
       </c>
@@ -2529,11 +2529,11 @@
       <c r="L73" s="1"/>
     </row>
     <row r="74" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A74" s="30"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="29"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="15"/>
       <c r="F74" s="6" t="s">
         <v>19</v>
       </c>
@@ -2549,11 +2549,11 @@
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A75" s="30"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="29"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="15"/>
       <c r="F75" s="6" t="s">
         <v>20</v>
       </c>
@@ -2569,19 +2569,19 @@
       <c r="L75" s="1"/>
     </row>
     <row r="76" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E76" s="29" t="s">
+      <c r="E76" s="15" t="s">
         <v>63</v>
       </c>
       <c r="F76" s="6" t="s">
@@ -2599,11 +2599,11 @@
       <c r="L76" s="1"/>
     </row>
     <row r="77" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A77" s="30"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="29"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="15"/>
       <c r="F77" s="6" t="s">
         <v>18</v>
       </c>
@@ -2619,11 +2619,11 @@
       <c r="L77" s="1"/>
     </row>
     <row r="78" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A78" s="30"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="29"/>
+      <c r="A78" s="16"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="15"/>
       <c r="F78" s="6" t="s">
         <v>19</v>
       </c>
@@ -2639,11 +2639,11 @@
       <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A79" s="30"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="29"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="15"/>
       <c r="F79" s="6" t="s">
         <v>20</v>
       </c>
@@ -2659,19 +2659,19 @@
       <c r="L79" s="1"/>
     </row>
     <row r="80" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D80" s="19" t="s">
+      <c r="D80" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E80" s="28" t="s">
+      <c r="E80" s="20" t="s">
         <v>68</v>
       </c>
       <c r="F80" s="6" t="s">
@@ -2689,11 +2689,11 @@
       <c r="L80" s="1"/>
     </row>
     <row r="81" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A81" s="30"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="28"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="20"/>
       <c r="F81" s="6" t="s">
         <v>18</v>
       </c>
@@ -2709,11 +2709,11 @@
       <c r="L81" s="1"/>
     </row>
     <row r="82" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A82" s="30"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="28"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="20"/>
       <c r="F82" s="6" t="s">
         <v>19</v>
       </c>
@@ -2729,11 +2729,11 @@
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A83" s="30"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="26"/>
-      <c r="E83" s="28"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="20"/>
       <c r="F83" s="6" t="s">
         <v>20</v>
       </c>
@@ -2749,19 +2749,19 @@
       <c r="L83" s="1"/>
     </row>
     <row r="84" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B84" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D84" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E84" s="29" t="s">
+      <c r="E84" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F84" s="6" t="s">
@@ -2779,11 +2779,11 @@
       <c r="L84" s="1"/>
     </row>
     <row r="85" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A85" s="30"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="26"/>
-      <c r="E85" s="29"/>
+      <c r="A85" s="16"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="15"/>
       <c r="F85" s="6" t="s">
         <v>18</v>
       </c>
@@ -2799,11 +2799,11 @@
       <c r="L85" s="1"/>
     </row>
     <row r="86" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A86" s="30"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="29"/>
+      <c r="A86" s="16"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="15"/>
       <c r="F86" s="6" t="s">
         <v>19</v>
       </c>
@@ -2819,11 +2819,11 @@
       <c r="L86" s="1"/>
     </row>
     <row r="87" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A87" s="30"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="29"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="15"/>
       <c r="F87" s="6" t="s">
         <v>20</v>
       </c>
@@ -2839,19 +2839,19 @@
       <c r="L87" s="1"/>
     </row>
     <row r="88" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A88" s="30" t="s">
+      <c r="A88" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C88" s="21" t="s">
+      <c r="C88" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E88" s="29" t="s">
+      <c r="E88" s="15" t="s">
         <v>74</v>
       </c>
       <c r="F88" s="6" t="s">
@@ -2869,11 +2869,11 @@
       <c r="L88" s="1"/>
     </row>
     <row r="89" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A89" s="30"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="29"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="15"/>
       <c r="F89" s="6" t="s">
         <v>18</v>
       </c>
@@ -2889,11 +2889,11 @@
       <c r="L89" s="1"/>
     </row>
     <row r="90" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A90" s="30"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="26"/>
-      <c r="E90" s="29"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="15"/>
       <c r="F90" s="6" t="s">
         <v>19</v>
       </c>
@@ -2909,11 +2909,11 @@
       <c r="L90" s="1"/>
     </row>
     <row r="91" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A91" s="30"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="29"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="15"/>
       <c r="F91" s="6" t="s">
         <v>20</v>
       </c>
@@ -2929,19 +2929,19 @@
       <c r="L91" s="1"/>
     </row>
     <row r="92" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A92" s="30" t="s">
+      <c r="A92" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="C92" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E92" s="29" t="s">
+      <c r="E92" s="15" t="s">
         <v>77</v>
       </c>
       <c r="F92" s="6" t="s">
@@ -2959,11 +2959,11 @@
       <c r="L92" s="1"/>
     </row>
     <row r="93" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A93" s="30"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="29"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="15"/>
       <c r="F93" s="6" t="s">
         <v>18</v>
       </c>
@@ -2979,11 +2979,11 @@
       <c r="L93" s="1"/>
     </row>
     <row r="94" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A94" s="30"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="26"/>
-      <c r="E94" s="29"/>
+      <c r="A94" s="16"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="15"/>
       <c r="F94" s="6" t="s">
         <v>19</v>
       </c>
@@ -2999,11 +2999,11 @@
       <c r="L94" s="1"/>
     </row>
     <row r="95" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A95" s="30"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="29"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="15"/>
       <c r="F95" s="6" t="s">
         <v>20</v>
       </c>
@@ -3019,19 +3019,19 @@
       <c r="L95" s="1"/>
     </row>
     <row r="96" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A96" s="30" t="s">
+      <c r="A96" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C96" s="25" t="s">
+      <c r="C96" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D96" s="19" t="s">
+      <c r="D96" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E96" s="22" t="s">
+      <c r="E96" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F96" s="6" t="s">
@@ -3049,11 +3049,11 @@
       <c r="L96" s="1"/>
     </row>
     <row r="97" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A97" s="30"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="23"/>
+      <c r="A97" s="16"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="22"/>
       <c r="F97" s="6" t="s">
         <v>18</v>
       </c>
@@ -3069,11 +3069,11 @@
       <c r="L97" s="1"/>
     </row>
     <row r="98" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A98" s="30"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="23"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="22"/>
       <c r="F98" s="6" t="s">
         <v>19</v>
       </c>
@@ -3089,11 +3089,11 @@
       <c r="L98" s="1"/>
     </row>
     <row r="99" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A99" s="30"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="26"/>
-      <c r="E99" s="23"/>
+      <c r="A99" s="16"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="22"/>
       <c r="F99" s="6" t="s">
         <v>20</v>
       </c>
@@ -3110,98 +3110,16 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="E88:E91"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="C24:C27"/>
@@ -3226,16 +3144,98 @@
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="D28:D31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D24" r:id="rId1" xr:uid="{E7CF1D17-3DF8-4EC5-B2CD-15F9F0A5DCCA}"/>

</xml_diff>